<commit_message>
A planilha de riscos para incrementar
</commit_message>
<xml_diff>
--- a/Documentação/planilha risco.xlsx
+++ b/Documentação/planilha risco.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/450d1bbef5244860/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\OneDrive\Desktop\Synergy\segunda-sprint\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="8_{7351757E-761E-46CC-8499-53D45927C721}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1BB29074-72B5-43DA-BD7D-04BE73B7DD24}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE6DC43B-E55A-4EBA-A5AA-F6CA739D3F04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{E9883AE3-2F29-46FF-B0B9-86C08474EE92}"/>
+    <workbookView xWindow="-2760" yWindow="2910" windowWidth="14400" windowHeight="15600" xr2:uid="{E9883AE3-2F29-46FF-B0B9-86C08474EE92}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Risco Indentificado</t>
   </si>
@@ -87,24 +87,6 @@
   </si>
   <si>
     <t>3º</t>
-  </si>
-  <si>
-    <t>Falha na leitura do sensor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bloqueio no leitor </t>
-  </si>
-  <si>
-    <t>alto</t>
-  </si>
-  <si>
-    <t>A não captação de dados</t>
-  </si>
-  <si>
-    <t>mudar posição</t>
-  </si>
-  <si>
-    <t>Id sensor</t>
   </si>
   <si>
     <t>Linha:</t>
@@ -363,6 +345,51 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -372,61 +399,16 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -746,7 +728,7 @@
   <dimension ref="B2:O11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="96" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="J4" sqref="J4:L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -765,22 +747,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="32"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="31"/>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B3" s="12"/>
@@ -799,31 +781,31 @@
       <c r="O3" s="13"/>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="20"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="K4" s="23"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="23" t="s">
+      <c r="B4" s="24"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="37" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4" s="37"/>
+      <c r="L4" s="37"/>
+      <c r="M4" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="N4" s="23"/>
-      <c r="O4" s="23"/>
+      <c r="N4" s="37"/>
+      <c r="O4" s="37"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="27"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -835,52 +817,50 @@
       <c r="O5" s="4"/>
     </row>
     <row r="6" spans="2:15" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="38" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="25" t="s">
+      <c r="B6" s="22"/>
+      <c r="C6" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="25" t="s">
+      <c r="E6" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="25" t="s">
+      <c r="F6" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="25" t="s">
+      <c r="G6" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="25"/>
-      <c r="I6" s="25" t="s">
+      <c r="H6" s="23"/>
+      <c r="I6" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="J6" s="22" t="s">
+      <c r="J6" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="K6" s="22"/>
-      <c r="L6" s="22"/>
-      <c r="M6" s="22" t="s">
+      <c r="K6" s="35"/>
+      <c r="L6" s="35"/>
+      <c r="M6" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="N6" s="22"/>
-      <c r="O6" s="22"/>
+      <c r="N6" s="35"/>
+      <c r="O6" s="35"/>
     </row>
     <row r="7" spans="2:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="B7" s="25"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
       <c r="G7" s="5" t="s">
         <v>7</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I7" s="26"/>
+      <c r="I7" s="38"/>
       <c r="J7" s="7" t="s">
         <v>11</v>
       </c>
@@ -900,26 +880,16 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="2:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="B8" s="29"/>
-      <c r="C8" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>19</v>
-      </c>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B8" s="19"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
       <c r="E8" s="14"/>
-      <c r="F8" s="14" t="s">
-        <v>20</v>
-      </c>
+      <c r="F8" s="14"/>
       <c r="G8" s="14"/>
       <c r="H8" s="14"/>
-      <c r="I8" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="J8" s="15" t="s">
-        <v>22</v>
-      </c>
+      <c r="I8" s="14"/>
+      <c r="J8" s="15"/>
       <c r="K8" s="15"/>
       <c r="L8" s="15"/>
       <c r="M8" s="7"/>
@@ -927,7 +897,7 @@
       <c r="O8" s="8"/>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B9" s="29"/>
+      <c r="B9" s="19"/>
       <c r="C9" s="16"/>
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
@@ -943,7 +913,7 @@
       <c r="O9" s="8"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B10" s="28"/>
+      <c r="B10" s="18"/>
       <c r="C10" s="16"/>
       <c r="D10" s="14"/>
       <c r="E10" s="14"/>
@@ -959,14 +929,14 @@
       <c r="O10" s="8"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="28"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="19"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="34"/>
       <c r="J11" s="9"/>
       <c r="K11" s="10"/>
       <c r="L11" s="11"/>

</xml_diff>